<commit_message>
Calculate confidence intervals when the population variance is unknown
</commit_message>
<xml_diff>
--- a/part3_statistics/data/ConfidenceIntervalsExercise_PopulationVarianceKnown.xlsx
+++ b/part3_statistics/data/ConfidenceIntervalsExercise_PopulationVarianceKnown.xlsx
@@ -204,7 +204,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -232,7 +232,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -321,7 +321,7 @@
   <sheetFormatPr defaultRowHeight="11.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.22"/>

</xml_diff>